<commit_message>
Learn C++: 03.03: 내용 추가
</commit_message>
<xml_diff>
--- a/asset/calendar.xlsx
+++ b/asset/calendar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adun/Desktop/여름방학 폐관수련/asset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95404107-EE94-C343-9E66-5FE24715020F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C5646A-CAFC-9842-AF86-C117E15F5CC6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="28800" windowHeight="16000" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -18999,7 +18999,7 @@
   </sheetPr>
   <dimension ref="A1:AA33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="156" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScale="156" workbookViewId="0">
       <selection activeCell="I27" sqref="I27:J27"/>
     </sheetView>
   </sheetViews>

</xml_diff>